<commit_message>
greatly improved mesh refinement, increased resources requested
</commit_message>
<xml_diff>
--- a/FDTR_Simulation_Fourier/Integral_Transform_Inversion/error_surface_data_concentric.xlsx
+++ b/FDTR_Simulation_Fourier/Integral_Transform_Inversion/error_surface_data_concentric.xlsx
@@ -435,2944 +435,2944 @@
   <sheetData>
     <row r="1">
       <c r="B1" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>9.896551724137931</v>
+        <v>101.7241379310345</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>18.79310344827586</v>
+        <v>103.448275862069</v>
       </c>
       <c r="E1" s="1" t="n">
-        <v>27.68965517241379</v>
+        <v>105.1724137931034</v>
       </c>
       <c r="F1" s="1" t="n">
-        <v>36.58620689655172</v>
+        <v>106.8965517241379</v>
       </c>
       <c r="G1" s="1" t="n">
-        <v>45.48275862068965</v>
+        <v>108.6206896551724</v>
       </c>
       <c r="H1" s="1" t="n">
-        <v>54.37931034482759</v>
+        <v>110.3448275862069</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>63.27586206896552</v>
+        <v>112.0689655172414</v>
       </c>
       <c r="J1" s="1" t="n">
-        <v>72.17241379310344</v>
+        <v>113.7931034482759</v>
       </c>
       <c r="K1" s="1" t="n">
-        <v>81.06896551724138</v>
+        <v>115.5172413793103</v>
       </c>
       <c r="L1" s="1" t="n">
-        <v>89.9655172413793</v>
+        <v>117.2413793103448</v>
       </c>
       <c r="M1" s="1" t="n">
-        <v>98.86206896551724</v>
+        <v>118.9655172413793</v>
       </c>
       <c r="N1" s="1" t="n">
-        <v>107.7586206896552</v>
+        <v>120.6896551724138</v>
       </c>
       <c r="O1" s="1" t="n">
-        <v>116.6551724137931</v>
+        <v>122.4137931034483</v>
       </c>
       <c r="P1" s="1" t="n">
-        <v>125.551724137931</v>
+        <v>124.1379310344828</v>
       </c>
       <c r="Q1" s="1" t="n">
-        <v>134.448275862069</v>
+        <v>125.8620689655172</v>
       </c>
       <c r="R1" s="1" t="n">
-        <v>143.3448275862069</v>
+        <v>127.5862068965517</v>
       </c>
       <c r="S1" s="1" t="n">
-        <v>152.2413793103448</v>
+        <v>129.3103448275862</v>
       </c>
       <c r="T1" s="1" t="n">
-        <v>161.1379310344828</v>
+        <v>131.0344827586207</v>
       </c>
       <c r="U1" s="1" t="n">
-        <v>170.0344827586207</v>
+        <v>132.7586206896552</v>
       </c>
       <c r="V1" s="1" t="n">
-        <v>178.9310344827586</v>
+        <v>134.4827586206897</v>
       </c>
       <c r="W1" s="1" t="n">
-        <v>187.8275862068965</v>
+        <v>136.2068965517241</v>
       </c>
       <c r="X1" s="1" t="n">
-        <v>196.7241379310345</v>
+        <v>137.9310344827586</v>
       </c>
       <c r="Y1" s="1" t="n">
-        <v>205.6206896551724</v>
+        <v>139.6551724137931</v>
       </c>
       <c r="Z1" s="1" t="n">
-        <v>214.5172413793103</v>
+        <v>141.3793103448276</v>
       </c>
       <c r="AA1" s="1" t="n">
-        <v>223.4137931034483</v>
+        <v>143.1034482758621</v>
       </c>
       <c r="AB1" s="1" t="n">
-        <v>232.3103448275862</v>
+        <v>144.8275862068965</v>
       </c>
       <c r="AC1" s="1" t="n">
-        <v>241.2068965517241</v>
+        <v>146.551724137931</v>
       </c>
       <c r="AD1" s="1" t="n">
-        <v>250.1034482758621</v>
+        <v>148.2758620689655</v>
       </c>
       <c r="AE1" s="1" t="n">
-        <v>259</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B2" t="n">
-        <v>1.160067946670854</v>
+        <v>0.002657665799476355</v>
       </c>
       <c r="C2" t="n">
-        <v>1.103037870762352</v>
+        <v>0.002509219975396184</v>
       </c>
       <c r="D2" t="n">
-        <v>1.056198440094654</v>
+        <v>0.002367690079446124</v>
       </c>
       <c r="E2" t="n">
-        <v>1.016152240613825</v>
+        <v>0.002232783165930221</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9810472869304027</v>
+        <v>0.002104221630023936</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9497453635964701</v>
+        <v>0.001981742223906515</v>
       </c>
       <c r="H2" t="n">
-        <v>0.921483221123153</v>
+        <v>0.001865095148013746</v>
       </c>
       <c r="I2" t="n">
-        <v>0.895717853892975</v>
+        <v>0.001754043210754193</v>
       </c>
       <c r="J2" t="n">
-        <v>0.8720461032032524</v>
+        <v>0.001648361050702668</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8501587997006955</v>
+        <v>0.001547834415879463</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8298127381859726</v>
+        <v>0.001452259495253815</v>
       </c>
       <c r="M2" t="n">
-        <v>0.810812617760845</v>
+        <v>0.001361442298079578</v>
       </c>
       <c r="N2" t="n">
-        <v>0.792998903828663</v>
+        <v>0.001275198077092592</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7762393860489619</v>
+        <v>0.0011933507919727</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7604231374152053</v>
+        <v>0.001115732609809829</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.7454560863055387</v>
+        <v>0.001042183439613265</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7312577032130104</v>
+        <v>0.0009725504981730406</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7177584767894986</v>
+        <v>0.0009066879048239841</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7048979607668598</v>
+        <v>0.0008444563028809288</v>
       </c>
       <c r="U2" t="n">
-        <v>0.6926232415143394</v>
+        <v>0.0007857225057093321</v>
       </c>
       <c r="V2" t="n">
-        <v>0.6808877206736771</v>
+        <v>0.0007303591655722987</v>
       </c>
       <c r="W2" t="n">
-        <v>0.6696501372941623</v>
+        <v>0.0006782444635546204</v>
       </c>
       <c r="X2" t="n">
-        <v>0.6588737744355591</v>
+        <v>0.0006292618190086515</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.6485258095552424</v>
+        <v>0.0005832996170971937</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.6385767781881379</v>
+        <v>0.0005402509531269804</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.6290001277803626</v>
+        <v>0.0005000133924737209</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.6197718439159842</v>
+        <v>0.0004624887449965253</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.6108701351615553</v>
+        <v>0.0004275828529289339</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.6022751657409819</v>
+        <v>0.0003952053913134617</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.5939688275176873</v>
+        <v>0.0003652696801205864</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>9.896551724137931</v>
+        <v>101.7241379310345</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4663478802940563</v>
+        <v>0.002447486963587381</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4037840042675999</v>
+        <v>0.002305475373758682</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3594977520082986</v>
+        <v>0.002170238878425615</v>
       </c>
       <c r="E3" t="n">
-        <v>0.3255320589682401</v>
+        <v>0.002041489119569817</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2981921496002685</v>
+        <v>0.001918952876279925</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2754782441291609</v>
+        <v>0.001802371092424125</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2561781069107928</v>
+        <v>0.001691497978647321</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2394982493800146</v>
+        <v>0.001586100182100945</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2248898313006673</v>
+        <v>0.001485956017977528</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2119571109217862</v>
+        <v>0.001390854757511869</v>
       </c>
       <c r="L3" t="n">
-        <v>0.2004052976107956</v>
+        <v>0.001300595967635388</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1900089653817248</v>
+        <v>0.001214988897936063</v>
       </c>
       <c r="N3" t="n">
-        <v>0.1805919644535346</v>
+        <v>0.001133851910992817</v>
       </c>
       <c r="O3" t="n">
-        <v>0.172014128419733</v>
+        <v>0.001057011952524775</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1641621837049152</v>
+        <v>0.0009843040581274955</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.156943357572068</v>
+        <v>0.0009155708936664031</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1502807753371168</v>
+        <v>0.0008506623266640193</v>
       </c>
       <c r="S3" t="n">
-        <v>0.1441100768938453</v>
+        <v>0.0007894350262573826</v>
       </c>
       <c r="T3" t="n">
-        <v>0.1383768842290175</v>
+        <v>0.0007317520895177243</v>
       </c>
       <c r="U3" t="n">
-        <v>0.1330348754216299</v>
+        <v>0.0006774826921180239</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1280442989450691</v>
+        <v>0.0006265017615098451</v>
       </c>
       <c r="W3" t="n">
-        <v>0.1233708129427155</v>
+        <v>0.0005786896709277584</v>
       </c>
       <c r="X3" t="n">
-        <v>0.1189845679328048</v>
+        <v>0.0005339319526835406</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.1148594743126259</v>
+        <v>0.0004921190293406541</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.1109726118644464</v>
+        <v>0.0004531459614770712</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.107303749590023</v>
+        <v>0.0004169122108503133</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1038349521373571</v>
+        <v>0.0003833214178755171</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.1005502548255563</v>
+        <v>0.0003522811924142807</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.09743539348157268</v>
+        <v>0.000323702916952283</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.09447757842278239</v>
+        <v>0.0002975015613161833</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>18.79310344827586</v>
+        <v>103.448275862069</v>
       </c>
       <c r="B4" t="n">
-        <v>0.3151428463726722</v>
+        <v>0.002250619825535537</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2599601057994801</v>
+        <v>0.002114847448090316</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2230973304508229</v>
+        <v>0.001985713084366109</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1959980643599219</v>
+        <v>0.001862932852290919</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1748923494763737</v>
+        <v>0.001746237807730001</v>
       </c>
       <c r="G4" t="n">
-        <v>0.157828261131202</v>
+        <v>0.001635372983455971</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1436635552727168</v>
+        <v>0.001530096501663887</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1316718941442128</v>
+        <v>0.001430178753502376</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1213630303650007</v>
+        <v>0.001335401639750312</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1123908725920425</v>
+        <v>0.001245557867353396</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1045023741278712</v>
+        <v>0.001160450297054263</v>
       </c>
       <c r="M4" t="n">
-        <v>0.09750722512927462</v>
+        <v>0.001079891337811884</v>
       </c>
       <c r="N4" t="n">
-        <v>0.09125893776807555</v>
+        <v>0.001003702384118685</v>
       </c>
       <c r="O4" t="n">
-        <v>0.08564254025139525</v>
+        <v>0.0009317132926911865</v>
       </c>
       <c r="P4" t="n">
-        <v>0.08056628934970965</v>
+        <v>0.0008637618953395244</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.0759559242164464</v>
+        <v>0.0007996935451159309</v>
       </c>
       <c r="R4" t="n">
-        <v>0.07175058166640962</v>
+        <v>0.0007393606931060674</v>
       </c>
       <c r="S4" t="n">
-        <v>0.06789982915680058</v>
+        <v>0.0006826224934651554</v>
       </c>
       <c r="T4" t="n">
-        <v>0.06436146854974099</v>
+        <v>0.0006293444345134742</v>
       </c>
       <c r="U4" t="n">
-        <v>0.06109988309808687</v>
+        <v>0.0005793979938988344</v>
       </c>
       <c r="V4" t="n">
-        <v>0.05808477471049165</v>
+        <v>0.0005326603160061211</v>
       </c>
       <c r="W4" t="n">
-        <v>0.05529018645763102</v>
+        <v>0.0004890139099509048</v>
       </c>
       <c r="X4" t="n">
-        <v>0.05269373677878404</v>
+        <v>0.0004483463666351828</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.05027601300141297</v>
+        <v>0.0004105500934715759</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.04802008626705198</v>
+        <v>0.0003755220654976364</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.0459111200425258</v>
+        <v>0.0003431635917075832</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.04393605153147618</v>
+        <v>0.0003133800955238675</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.04208333042313787</v>
+        <v>0.0002860809084177294</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.04034270314043329</v>
+        <v>0.0002611790757669933</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.03870503349174102</v>
+        <v>0.0002385911741110322</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>27.68965517241379</v>
+        <v>105.1724137931034</v>
       </c>
       <c r="B5" t="n">
-        <v>0.239332059731584</v>
+        <v>0.002066332786165881</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1901701739058572</v>
+        <v>0.0019366129781538</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1585601062805267</v>
+        <v>0.00181339770802612</v>
       </c>
       <c r="E5" t="n">
-        <v>0.135981734915395</v>
+        <v>0.001696407462033036</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1187930205883772</v>
+        <v>0.001585377469628485</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1051587308520826</v>
+        <v>0.001480056753503541</v>
       </c>
       <c r="H5" t="n">
-        <v>0.09402811232584515</v>
+        <v>0.001380207252400031</v>
       </c>
       <c r="I5" t="n">
-        <v>0.08474499447111621</v>
+        <v>0.001285603010237546</v>
       </c>
       <c r="J5" t="n">
-        <v>0.07687326866697249</v>
+        <v>0.001196029425739851</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0701091698621181</v>
+        <v>0.001111282557326362</v>
       </c>
       <c r="L5" t="n">
-        <v>0.06423322570953924</v>
+        <v>0.001031168478548583</v>
       </c>
       <c r="M5" t="n">
-        <v>0.05908213286818855</v>
+        <v>0.0009555026798099673</v>
       </c>
       <c r="N5" t="n">
-        <v>0.05453140836383347</v>
+        <v>0.0008841095125160718</v>
       </c>
       <c r="O5" t="n">
-        <v>0.05048422044539791</v>
+        <v>0.0008168216721659407</v>
       </c>
       <c r="P5" t="n">
-        <v>0.04686393823148182</v>
+        <v>0.0007534797172225713</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.04360901101680145</v>
+        <v>0.0006939316208915192</v>
       </c>
       <c r="R5" t="n">
-        <v>0.04066935751858029</v>
+        <v>0.0006380323531989048</v>
       </c>
       <c r="S5" t="n">
-        <v>0.03800376277699229</v>
+        <v>0.0005856434909951287</v>
       </c>
       <c r="T5" t="n">
-        <v>0.03557796478051752</v>
+        <v>0.0005366328537217349</v>
       </c>
       <c r="U5" t="n">
-        <v>0.03336322381100939</v>
+        <v>0.0004908741629697077</v>
       </c>
       <c r="V5" t="n">
-        <v>0.03133523633731378</v>
+        <v>0.0004482467240283968</v>
       </c>
       <c r="W5" t="n">
-        <v>0.02947329917945717</v>
+        <v>0.0004086351277798124</v>
       </c>
       <c r="X5" t="n">
-        <v>0.02775965833909367</v>
+        <v>0.0003719289714324872</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.02617899603233385</v>
+        <v>0.0003380225967159937</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.02471802248859136</v>
+        <v>0.0003068148442719428</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.02336514810327663</v>
+        <v>0.0002782088230812054</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.02211021788400428</v>
+        <v>0.0002521116938616282</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.02094429466659039</v>
+        <v>0.0002284344654563719</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.01985948086095032</v>
+        <v>0.0002070918033111241</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.01884877089348917</v>
+        <v>0.0001880018492094679</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>36.58620689655172</v>
+        <v>106.8965517241379</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1924671000770689</v>
+        <v>0.001893942218612168</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1481175416475844</v>
+        <v>0.001770096242789211</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1204172148541547</v>
+        <v>0.001652624793817378</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1010733340195598</v>
+        <v>0.001541252622548466</v>
       </c>
       <c r="F6" t="n">
-        <v>0.08661335726763777</v>
+        <v>0.001435719032590146</v>
       </c>
       <c r="G6" t="n">
-        <v>0.07532113742978624</v>
+        <v>0.00133577694117567</v>
       </c>
       <c r="H6" t="n">
-        <v>0.06622956363628597</v>
+        <v>0.001241192012063641</v>
       </c>
       <c r="I6" t="n">
-        <v>0.05874266678486072</v>
+        <v>0.001151741854062127</v>
       </c>
       <c r="J6" t="n">
-        <v>0.05246884580697643</v>
+        <v>0.001067215279418555</v>
       </c>
       <c r="K6" t="n">
-        <v>0.04713805634599009</v>
+        <v>0.0009874116168914655</v>
       </c>
       <c r="L6" t="n">
-        <v>0.04255692735610815</v>
+        <v>0.000912140074829349</v>
       </c>
       <c r="M6" t="n">
-        <v>0.03858273761042631</v>
+        <v>0.0008412191500371599</v>
       </c>
       <c r="N6" t="n">
-        <v>0.03510749776371191</v>
+        <v>0.0007744760786146498</v>
       </c>
       <c r="O6" t="n">
-        <v>0.03204778055918208</v>
+        <v>0.0007117463253126746</v>
       </c>
       <c r="P6" t="n">
-        <v>0.02933798448740341</v>
+        <v>0.0006528731082762941</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.02692573366263654</v>
+        <v>0.0005977069563330606</v>
       </c>
       <c r="R6" t="n">
-        <v>0.02476865352826963</v>
+        <v>0.0005461052962439601</v>
       </c>
       <c r="S6" t="n">
-        <v>0.02283205933760037</v>
+        <v>0.0004979320675674077</v>
       </c>
       <c r="T6" t="n">
-        <v>0.02108726599754334</v>
+        <v>0.0004530573629964186</v>
       </c>
       <c r="U6" t="n">
-        <v>0.0195103305547245</v>
+        <v>0.0004113570922169831</v>
       </c>
       <c r="V6" t="n">
-        <v>0.01808110199295743</v>
+        <v>0.0003727126675062649</v>
       </c>
       <c r="W6" t="n">
-        <v>0.01678249323203247</v>
+        <v>0.0003370107094420558</v>
       </c>
       <c r="X6" t="n">
-        <v>0.01559991636953335</v>
+        <v>0.000304142771233938</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.01452083958706912</v>
+        <v>0.000274005080311815</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.01353443592165338</v>
+        <v>0.0002464982959210253</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.01263130222988251</v>
+        <v>0.0002215272815764318</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.01180323237098413</v>
+        <v>0.0001990008913212189</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.01104303268986697</v>
+        <v>0.0001788317688212472</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.01034437080628052</v>
+        <v>0.0001609361584030262</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.00970165085249206</v>
+        <v>0.0001452337272138675</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45.48275862068965</v>
+        <v>108.6206896551724</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1602863325642572</v>
+        <v>0.001732808718038686</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1198644488545727</v>
+        <v>0.001614665302801675</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09520891183791935</v>
+        <v>0.001502769735325356</v>
       </c>
       <c r="E7" t="n">
-        <v>0.07831613807219924</v>
+        <v>0.001396850931055728</v>
       </c>
       <c r="F7" t="n">
-        <v>0.06588567070082241</v>
+        <v>0.001296652171888637</v>
       </c>
       <c r="G7" t="n">
-        <v>0.056310859188838</v>
+        <v>0.001201930177655867</v>
       </c>
       <c r="H7" t="n">
-        <v>0.04869753160077858</v>
+        <v>0.001112454248905411</v>
       </c>
       <c r="I7" t="n">
-        <v>0.04250045546935875</v>
+        <v>0.001028005474630268</v>
       </c>
       <c r="J7" t="n">
-        <v>0.03736463447154147</v>
+        <v>0.0009483759992416369</v>
       </c>
       <c r="K7" t="n">
-        <v>0.03304724331232969</v>
+        <v>0.0008733683436515485</v>
       </c>
       <c r="L7" t="n">
-        <v>0.02937566586452487</v>
+        <v>0.0008027947758358657</v>
       </c>
       <c r="M7" t="n">
-        <v>0.02622334473030863</v>
+        <v>0.000736476726698225</v>
       </c>
       <c r="N7" t="n">
-        <v>0.02349510720887109</v>
+        <v>0.000674244247456724</v>
       </c>
       <c r="O7" t="n">
-        <v>0.0211178470514531</v>
+        <v>0.0006159355051333943</v>
       </c>
       <c r="P7" t="n">
-        <v>0.01903438658421371</v>
+        <v>0.0005613963130461839</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.01719930691207575</v>
+        <v>0.0005104796934901395</v>
       </c>
       <c r="R7" t="n">
-        <v>0.01557603932177035</v>
+        <v>0.000463045470051314</v>
       </c>
       <c r="S7" t="n">
-        <v>0.01413478950520434</v>
+        <v>0.0004189598872275021</v>
       </c>
       <c r="T7" t="n">
-        <v>0.01285102623600172</v>
+        <v>0.0003780952552376613</v>
       </c>
       <c r="U7" t="n">
-        <v>0.01170436144318898</v>
+        <v>0.0003403296180881278</v>
       </c>
       <c r="V7" t="n">
-        <v>0.01067770721527215</v>
+        <v>0.0003055464431326941</v>
       </c>
       <c r="W7" t="n">
-        <v>0.009756632297500505</v>
+        <v>0.0002736343305147071</v>
       </c>
       <c r="X7" t="n">
-        <v>0.008928864632566281</v>
+        <v>0.0002444867410174793</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.008183902380188251</v>
+        <v>0.0002180017409728661</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.007512706581374981</v>
+        <v>0.0001940817629905613</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.00690745601264529</v>
+        <v>0.000172633381372657</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.006361349933967747</v>
+        <v>0.0001535671011706832</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.00586844809422688</v>
+        <v>0.0001367971599262697</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.005423539990616701</v>
+        <v>0.0001222413412132966</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.005022037295878208</v>
+        <v>0.0001098207991690471</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>54.37931034482759</v>
+        <v>110.3448275862069</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1367199056994217</v>
+        <v>0.001582333693365328</v>
       </c>
       <c r="C8" t="n">
-        <v>0.09957274182578806</v>
+        <v>0.001469728623065904</v>
       </c>
       <c r="D8" t="n">
-        <v>0.07736948393280421</v>
+        <v>0.001363247927321188</v>
       </c>
       <c r="E8" t="n">
-        <v>0.06241019056343894</v>
+        <v>0.001262624589698293</v>
       </c>
       <c r="F8" t="n">
-        <v>0.05155767596723634</v>
+        <v>0.001167605777912614</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04330351254882937</v>
+        <v>0.00107795192571728</v>
       </c>
       <c r="H8" t="n">
-        <v>0.03681682076731484</v>
+        <v>0.0009934358853647943</v>
       </c>
       <c r="I8" t="n">
-        <v>0.03159541224491255</v>
+        <v>0.0009138421443539967</v>
       </c>
       <c r="J8" t="n">
-        <v>0.02731483105815223</v>
+        <v>0.000838966100811838</v>
       </c>
       <c r="K8" t="n">
-        <v>0.02375466639205633</v>
+        <v>0.0007686133924234691</v>
       </c>
       <c r="L8" t="n">
-        <v>0.02075921221089353</v>
+        <v>0.0007025992743255428</v>
       </c>
       <c r="M8" t="n">
-        <v>0.01821496327921271</v>
+        <v>0.0006407480418234479</v>
       </c>
       <c r="N8" t="n">
-        <v>0.01603701701649195</v>
+        <v>0.0005828924941909687</v>
       </c>
       <c r="O8" t="n">
-        <v>0.01416048215301868</v>
+        <v>0.0005288734361653752</v>
       </c>
       <c r="P8" t="n">
-        <v>0.01253484612672476</v>
+        <v>0.0004785392140684165</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.01112016520916869</v>
+        <v>0.0004317452837675748</v>
       </c>
       <c r="R8" t="n">
-        <v>0.009884417809549776</v>
+        <v>0.0003883538079464472</v>
       </c>
       <c r="S8" t="n">
-        <v>0.008801622868144921</v>
+        <v>0.0003482332803819883</v>
       </c>
       <c r="T8" t="n">
-        <v>0.007850474888485158</v>
+        <v>0.0003112581751314531</v>
       </c>
       <c r="U8" t="n">
-        <v>0.007013335964455468</v>
+        <v>0.0002773086187171758</v>
       </c>
       <c r="V8" t="n">
-        <v>0.006275479561743499</v>
+        <v>0.000246270083563935</v>
       </c>
       <c r="W8" t="n">
-        <v>0.005624515085017872</v>
+        <v>0.0002180331010940685</v>
       </c>
       <c r="X8" t="n">
-        <v>0.005049944394689511</v>
+        <v>0.0001924929930215003</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.004542816050725202</v>
+        <v>0.00016954961950896</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.004095452904616859</v>
+        <v>0.0001491071429637203</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.003701235412050706</v>
+        <v>0.0001310738063486167</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.00335442774608083</v>
+        <v>0.000115361724976465</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.003050037122201461</v>
+        <v>0.0001018866908393796</v>
       </c>
       <c r="AD8" t="n">
-        <v>0.002783699137305356</v>
+        <v>9.056798860038576e-05</v>
       </c>
       <c r="AE8" t="n">
-        <v>0.002551583661738212</v>
+        <v>8.132822244360026e-05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>63.27586206896552</v>
+        <v>112.0689655172414</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1186889903515645</v>
+        <v>0.001441956265343964</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08432176044585092</v>
+        <v>0.00133473199848334</v>
       </c>
       <c r="D9" t="n">
-        <v>0.06414442478689306</v>
+        <v>0.001233511719163938</v>
       </c>
       <c r="E9" t="n">
-        <v>0.05075585639608921</v>
+        <v>0.001138032385967162</v>
       </c>
       <c r="F9" t="n">
-        <v>0.04117022260128861</v>
+        <v>0.001048044963194366</v>
       </c>
       <c r="G9" t="n">
-        <v>0.03396679846807585</v>
+        <v>0.0009633135129533533</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02836990173370386</v>
+        <v>0.0008836143571081373</v>
       </c>
       <c r="I9" t="n">
-        <v>0.02391426621323264</v>
+        <v>0.0008087353028635833</v>
       </c>
       <c r="J9" t="n">
-        <v>0.02030130677191876</v>
+        <v>0.0007384749263864993</v>
       </c>
       <c r="K9" t="n">
-        <v>0.01732941182770424</v>
+        <v>0.0006726419094245682</v>
       </c>
       <c r="L9" t="n">
-        <v>0.01485694213968466</v>
+        <v>0.0006110544243812436</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0127811748961699</v>
+        <v>0.0005535395637466155</v>
       </c>
       <c r="N9" t="n">
-        <v>0.01102564092491017</v>
+        <v>0.0004999328101787518</v>
       </c>
       <c r="O9" t="n">
-        <v>0.009532159275363546</v>
+        <v>0.000450077543881135</v>
       </c>
       <c r="P9" t="n">
-        <v>0.008255636182557303</v>
+        <v>0.0004038245842365543</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.007160560463983738</v>
+        <v>0.0003610317629390679</v>
       </c>
       <c r="R9" t="n">
-        <v>0.006218577596552139</v>
+        <v>0.0003215635261180515</v>
       </c>
       <c r="S9" t="n">
-        <v>0.005406770898324934</v>
+        <v>0.0002852905631746437</v>
       </c>
       <c r="T9" t="n">
-        <v>0.004706418663797366</v>
+        <v>0.000252089460254794</v>
       </c>
       <c r="U9" t="n">
-        <v>0.004102079180234064</v>
+        <v>0.0002218423764660118</v>
       </c>
       <c r="V9" t="n">
-        <v>0.003580906296629648</v>
+        <v>0.0001944367411104058</v>
       </c>
       <c r="W9" t="n">
-        <v>0.003132130094124448</v>
+        <v>0.0001697649703555195</v>
       </c>
       <c r="X9" t="n">
-        <v>0.002746657737786775</v>
+        <v>0.0001477242018990022</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.002416763111365018</v>
+        <v>0.0001282160463052918</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.002135842922490349</v>
+        <v>0.0001111463538024406</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.001898223182913297</v>
+        <v>9.642499542750148e-05</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.001699004293279591</v>
+        <v>8.396565749953824e-05</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.001533936016268252</v>
+        <v>7.368564848190429e-05</v>
       </c>
       <c r="AD9" t="n">
-        <v>0.001399315808938713</v>
+        <v>6.550571737038468e-05</v>
       </c>
       <c r="AE9" t="n">
-        <v>0.001291905571181442</v>
+        <v>5.934988281212905e-05</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>72.17241379310344</v>
+        <v>113.7931034482759</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1044464391355393</v>
+        <v>0.001311150439523616</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0724744816802281</v>
+        <v>0.001209155752567055</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05400431963830471</v>
+        <v>0.001113047638603193</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04192085395035939</v>
+        <v>0.001022566941329039</v>
       </c>
       <c r="F10" t="n">
-        <v>0.03337741797747563</v>
+        <v>0.0009374683354812305</v>
       </c>
       <c r="G10" t="n">
-        <v>0.02703174242456657</v>
+        <v>0.0008575194289191908</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0221566426913347</v>
+        <v>0.0007824999338760802</v>
       </c>
       <c r="I10" t="n">
-        <v>0.01831887634961966</v>
+        <v>0.0007122009012058215</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01524207496163856</v>
+        <v>0.0006464240120795809</v>
       </c>
       <c r="K10" t="n">
-        <v>0.01274064250608872</v>
+        <v>0.0005849809221399272</v>
       </c>
       <c r="L10" t="n">
-        <v>0.01068484438330635</v>
+        <v>0.0005276926536130337</v>
       </c>
       <c r="M10" t="n">
-        <v>0.008981031456790104</v>
+        <v>0.0004743890313180119</v>
       </c>
       <c r="N10" t="n">
-        <v>0.007559796709800014</v>
+        <v>0.0004249081589027437</v>
       </c>
       <c r="O10" t="n">
-        <v>0.006368554119157887</v>
+        <v>0.0003790959319841829</v>
       </c>
       <c r="P10" t="n">
-        <v>0.005366710515861184</v>
+        <v>0.000336805585182709</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.004522423293678802</v>
+        <v>0.0002978972703190277</v>
       </c>
       <c r="R10" t="n">
-        <v>0.003810363265209784</v>
+        <v>0.0002622376632920558</v>
       </c>
       <c r="S10" t="n">
-        <v>0.003210134434880819</v>
+        <v>0.0002296995973807149</v>
       </c>
       <c r="T10" t="n">
-        <v>0.002705134679759146</v>
+        <v>0.0002001617209142779</v>
       </c>
       <c r="U10" t="n">
-        <v>0.002281719341045648</v>
+        <v>0.0001735081774374192</v>
       </c>
       <c r="V10" t="n">
-        <v>0.00192857725478228</v>
+        <v>0.0001496283066599181</v>
       </c>
       <c r="W10" t="n">
-        <v>0.00163625853201808</v>
+        <v>0.0001284163646283687</v>
       </c>
       <c r="X10" t="n">
-        <v>0.00139681253479383</v>
+        <v>0.0001097712616909232</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.001203507068764788</v>
+        <v>9.359631694651347e-05</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.001050608244300578</v>
+        <v>7.979902797941529e-05</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.0009332062148326752</v>
+        <v>6.829085477903473e-05</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.0008470759979274837</v>
+        <v>5.898701683469037e-05</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.0007885654015749848</v>
+        <v>5.180630247685382e-05</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.0007545040914593378</v>
+        <v>4.667088961065563e-05</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.0007421292923369377</v>
+        <v>4.350617705503795e-05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>81.06896551724138</v>
+        <v>115.5172413793103</v>
       </c>
       <c r="B11" t="n">
-        <v>0.09291959184636307</v>
+        <v>0.001189422526271737</v>
       </c>
       <c r="C11" t="n">
-        <v>0.06303712843526041</v>
+        <v>0.001092512181034435</v>
       </c>
       <c r="D11" t="n">
-        <v>0.04602853821110199</v>
+        <v>0.001001373858571277</v>
       </c>
       <c r="E11" t="n">
-        <v>0.03504897190279617</v>
+        <v>0.0009157522008557253</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02737946413431783</v>
+        <v>0.0008354055098485532</v>
       </c>
       <c r="G11" t="n">
-        <v>0.02174821866801155</v>
+        <v>0.0007601048593836079</v>
       </c>
       <c r="H11" t="n">
-        <v>0.01747099199618</v>
+        <v>0.0006896332755382333</v>
       </c>
       <c r="I11" t="n">
-        <v>0.01414259917662575</v>
+        <v>0.0006237849793730518</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01150597808014112</v>
+        <v>0.0005623646865448037</v>
       </c>
       <c r="K11" t="n">
-        <v>0.009389358111262829</v>
+        <v>0.0005051869588466677</v>
       </c>
       <c r="L11" t="n">
-        <v>0.00767322444508626</v>
+        <v>0.0004520756032181767</v>
       </c>
       <c r="M11" t="n">
-        <v>0.006271680466027224</v>
+        <v>0.0004028631142017861</v>
       </c>
       <c r="N11" t="n">
-        <v>0.005121328049850455</v>
+        <v>0.0003573901562100598</v>
       </c>
       <c r="O11" t="n">
-        <v>0.004174324185057786</v>
+        <v>0.0003155050823130066</v>
       </c>
       <c r="P11" t="n">
-        <v>0.003393878439316813</v>
+        <v>0.0002770634865640471</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.002751238670853211</v>
+        <v>0.0002419277871592491</v>
       </c>
       <c r="R11" t="n">
-        <v>0.002223617310113253</v>
+        <v>0.0002099668379724966</v>
       </c>
       <c r="S11" t="n">
-        <v>0.001792730676810766</v>
+        <v>0.0001810555662315579</v>
       </c>
       <c r="T11" t="n">
-        <v>0.001443748683226012</v>
+        <v>0.0001550746342998916</v>
       </c>
       <c r="U11" t="n">
-        <v>0.001164525778470347</v>
+        <v>0.0001319101237089207</v>
       </c>
       <c r="V11" t="n">
-        <v>0.0009450286635469094</v>
+        <v>0.0001114532397477881</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0007769042402631323</v>
+        <v>9.360003506370034e-05</v>
       </c>
       <c r="X11" t="n">
-        <v>0.0006531491672172847</v>
+        <v>7.825115085817902e-05</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.0005678541408816476</v>
+        <v>6.531157438416908e-05</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.0005160038790216478</v>
+        <v>5.469041155705285e-05</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.0004933191399611518</v>
+        <v>4.630067359074164e-05</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.0004961308228992757</v>
+        <v>4.005907665919022e-05</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.0005212788059316345</v>
+        <v>3.588585366445702e-05</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.0005660300415479098</v>
+        <v>3.370457726602745e-05</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.0006280117757577236</v>
+        <v>3.344199339318776e-05</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>89.9655172413793</v>
+        <v>117.2413793103448</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0834101641597504</v>
+        <v>0.001076308783184515</v>
       </c>
       <c r="C12" t="n">
-        <v>0.05536947801063382</v>
+        <v>0.000984343215929792</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03962855341260883</v>
+        <v>0.0008980378826743</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02959631231103498</v>
+        <v>0.0008171411397482423</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02267105251380617</v>
+        <v>0.0007414148359301938</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01764458485901901</v>
+        <v>0.0006706334339468435</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01387096490755688</v>
+        <v>0.0006045831997871307</v>
       </c>
       <c r="I12" t="n">
-        <v>0.01096981186034757</v>
+        <v>0.0005430614537697785</v>
       </c>
       <c r="J12" t="n">
-        <v>0.008701013240269985</v>
+        <v>0.0004858758779185042</v>
       </c>
       <c r="K12" t="n">
-        <v>0.006904867665200843</v>
+        <v>0.0004328438747439193</v>
       </c>
       <c r="L12" t="n">
-        <v>0.005470739471351265</v>
+        <v>0.0003837919730157014</v>
       </c>
       <c r="M12" t="n">
-        <v>0.004319440036680417</v>
+        <v>0.0003385552765392582</v>
       </c>
       <c r="N12" t="n">
-        <v>0.003392751881118891</v>
+        <v>0.0002969769523348054</v>
       </c>
       <c r="O12" t="n">
-        <v>0.00264690819921407</v>
+        <v>0.0002589077549596169</v>
       </c>
       <c r="P12" t="n">
-        <v>0.002048377296797963</v>
+        <v>0.0002242055840198957</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.001571048476694457</v>
+        <v>0.0001927350721930684</v>
       </c>
       <c r="R12" t="n">
-        <v>0.001194301307087319</v>
+        <v>0.0001643672013266412</v>
       </c>
       <c r="S12" t="n">
-        <v>0.0009016492089488856</v>
+        <v>0.0001389789444003073</v>
       </c>
       <c r="T12" t="n">
-        <v>0.0006797665902681665</v>
+        <v>0.0001164529313359847</v>
       </c>
       <c r="U12" t="n">
-        <v>0.0005177782230669847</v>
+        <v>9.667713681883154e-05</v>
       </c>
       <c r="V12" t="n">
-        <v>0.0004067316921458844</v>
+        <v>7.954458845288005e-05</v>
       </c>
       <c r="W12" t="n">
-        <v>0.0003392000348203</v>
+        <v>6.495309371989282e-05</v>
       </c>
       <c r="X12" t="n">
-        <v>0.0003089785148318887</v>
+        <v>5.280498434092311e-05</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.0003108504853867741</v>
+        <v>4.300687675860243e-05</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.0003404046515972489</v>
+        <v>3.546944756520139e-05</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.0003938910466473348</v>
+        <v>3.010722279886565e-05</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.0004681064977021791</v>
+        <v>2.683838011858929e-05</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.0005603027890961913</v>
+        <v>2.558456294852346e-05</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.0006681124622768422</v>
+        <v>2.627070575524877e-05</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.0007894884415893122</v>
+        <v>2.882486968782375e-05</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>98.86206896551724</v>
+        <v>118.9655172413793</v>
       </c>
       <c r="B13" t="n">
-        <v>0.07544246392561275</v>
+        <v>0.000971373257985649</v>
       </c>
       <c r="C13" t="n">
-        <v>0.04903961608895604</v>
+        <v>0.0008842182885465457</v>
       </c>
       <c r="D13" t="n">
-        <v>0.03441016573861625</v>
+        <v>0.0008026144278191333</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02520069673708445</v>
+        <v>0.0007263136653580814</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01891739592049044</v>
+        <v>0.0006550813190309182</v>
       </c>
       <c r="G13" t="n">
-        <v>0.01440976345813715</v>
+        <v>0.0005886951659490937</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01106624208249182</v>
+        <v>0.000526944640554667</v>
       </c>
       <c r="I13" t="n">
-        <v>0.008528553290785753</v>
+        <v>0.0004696300938560336</v>
       </c>
       <c r="J13" t="n">
-        <v>0.006571597551258647</v>
+        <v>0.0004165621084157196</v>
       </c>
       <c r="K13" t="n">
-        <v>0.005046311018769806</v>
+        <v>0.000367560864233787</v>
       </c>
       <c r="L13" t="n">
-        <v>0.003849851355300409</v>
+        <v>0.0003224555511508529</v>
       </c>
       <c r="M13" t="n">
-        <v>0.002908896434621709</v>
+        <v>0.0002810838238214835</v>
       </c>
       <c r="N13" t="n">
-        <v>0.00216974519495693</v>
+        <v>0.0002432912956894439</v>
       </c>
       <c r="O13" t="n">
-        <v>0.001592174389046033</v>
+        <v>0.0002089310687359247</v>
       </c>
       <c r="P13" t="n">
-        <v>0.001145478019682693</v>
+        <v>0.0001778632960750767</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0008058305056103924</v>
+        <v>0.0001499547747429293</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0005544822059826963</v>
+        <v>0.0001250785662692974</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0003764948302727647</v>
+        <v>0.0001031136428403491</v>
       </c>
       <c r="T13" t="n">
-        <v>0.000259836592899671</v>
+        <v>8.394455705630611e-05</v>
       </c>
       <c r="U13" t="n">
-        <v>0.0001947228063260277</v>
+        <v>6.746113346503219e-05</v>
       </c>
       <c r="V13" t="n">
-        <v>0.0001731274576115805</v>
+        <v>5.355818021174064e-05</v>
       </c>
       <c r="W13" t="n">
-        <v>0.0001884161334032562</v>
+        <v>4.213521928842554e-05</v>
       </c>
       <c r="X13" t="n">
-        <v>0.0002350665127016848</v>
+        <v>3.309623399656858e-05</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.000308453005802954</v>
+        <v>2.63494323538238e-05</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.0004046790254694462</v>
+        <v>2.180702528168718e-05</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.0005204450681517061</v>
+        <v>1.938501850740762e-05</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.0006529440235713917</v>
+        <v>1.900301720079657e-05</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.0007997774035648713</v>
+        <v>2.058404244591384e-05</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.0009588877973624003</v>
+        <v>2.405435871982413e-05</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.001128504024895432</v>
+        <v>2.934331161631107e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>107.7586206896552</v>
+        <v>120.6896551724138</v>
       </c>
       <c r="B14" t="n">
-        <v>0.06868045259817962</v>
+        <v>0.000874205812436281</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0437452102143981</v>
+        <v>0.0007917323718236374</v>
       </c>
       <c r="D14" t="n">
-        <v>0.03009929250262802</v>
+        <v>0.0007147034848008273</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02161168690685415</v>
+        <v>0.0006428746956775831</v>
       </c>
       <c r="F14" t="n">
-        <v>0.01588809422611462</v>
+        <v>0.0005760147162393507</v>
       </c>
       <c r="G14" t="n">
-        <v>0.01183058094488782</v>
+        <v>0.0005139045659319972</v>
       </c>
       <c r="H14" t="n">
-        <v>0.008858651162317587</v>
+        <v>0.0004563367785553278</v>
       </c>
       <c r="I14" t="n">
-        <v>0.006633859165462671</v>
+        <v>0.000403114669511735</v>
       </c>
       <c r="J14" t="n">
-        <v>0.004944505832252395</v>
+        <v>0.0003540516582614338</v>
       </c>
       <c r="K14" t="n">
-        <v>0.003650980927463228</v>
+        <v>0.000308970641171428</v>
       </c>
       <c r="L14" t="n">
-        <v>0.002657342448479869</v>
+        <v>0.0002677034104217544</v>
       </c>
       <c r="M14" t="n">
-        <v>0.001895445895687925</v>
+        <v>0.0002300901150560333</v>
       </c>
       <c r="N14" t="n">
-        <v>0.001315565008058563</v>
+        <v>0.0001959787606405521</v>
       </c>
       <c r="O14" t="n">
-        <v>0.0008805872518388025</v>
+        <v>0.0001652247443328856</v>
       </c>
       <c r="P14" t="n">
-        <v>0.0005622814865336798</v>
+        <v>0.0001376904224618028</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.0003388193361078605</v>
+        <v>0.0001132447079894896</v>
       </c>
       <c r="R14" t="n">
-        <v>0.000193083088732935</v>
+        <v>9.176269546836345e-05</v>
       </c>
       <c r="S14" t="n">
-        <v>0.0001114826397823523</v>
+        <v>7.312531132135974e-05</v>
       </c>
       <c r="T14" t="n">
-        <v>8.311091367947307e-05</v>
+        <v>5.721898746899277e-05</v>
       </c>
       <c r="U14" t="n">
-        <v>9.912974489453213e-05</v>
+        <v>4.393535650183567e-05</v>
       </c>
       <c r="V14" t="n">
-        <v>0.0001523159895926604</v>
+        <v>3.317096675456989e-05</v>
       </c>
       <c r="W14" t="n">
-        <v>0.000236721135308829</v>
+        <v>2.48270157802395e-05</v>
       </c>
       <c r="X14" t="n">
-        <v>0.0003474126592410601</v>
+        <v>1.880910085184615e-05</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.0004802751596042098</v>
+        <v>1.502698523458808e-05</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.0006318557915566237</v>
+        <v>1.339437907743477e-05</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.0007992429520582023</v>
+        <v>1.38287338679515e-05</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.0009799702012601155</v>
+        <v>1.625104948096308e-05</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.001171939539132974</v>
+        <v>2.058569293020655e-05</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.001373359669499898</v>
+        <v>2.676022800362969e-05</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.001582695972438684</v>
+        <v>3.470525502807767e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>116.6551724137931</v>
+        <v>122.4137931034483</v>
       </c>
       <c r="B15" t="n">
-        <v>0.06287958205777165</v>
+        <v>0.0007844203099043143</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03926813910271591</v>
+        <v>0.000706504185001164</v>
       </c>
       <c r="D15" t="n">
-        <v>0.02649944719113293</v>
+        <v>0.0006339285397702836</v>
       </c>
       <c r="E15" t="n">
-        <v>0.01865067932787373</v>
+        <v>0.0005664523973524827</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01341957553181404</v>
+        <v>0.0005038477907246444</v>
       </c>
       <c r="G15" t="n">
-        <v>0.009756309936196412</v>
+        <v>0.0004458989119656851</v>
       </c>
       <c r="H15" t="n">
-        <v>0.007108596580527565</v>
+        <v>0.0003924013273957</v>
       </c>
       <c r="I15" t="n">
-        <v>0.005155896498924276</v>
+        <v>0.0003431612526870802</v>
       </c>
       <c r="J15" t="n">
-        <v>0.003698552770129307</v>
+        <v>0.0002979948826461195</v>
       </c>
       <c r="K15" t="n">
-        <v>0.002605417437070692</v>
+        <v>0.0002567277708955199</v>
       </c>
       <c r="L15" t="n">
-        <v>0.001786704691523228</v>
+        <v>0.0002191942551601461</v>
       </c>
       <c r="M15" t="n">
-        <v>0.001178875921934903</v>
+        <v>0.0001852369242786072</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0007357316916281963</v>
+        <v>0.0001547061234371022</v>
       </c>
       <c r="O15" t="n">
-        <v>0.0004229132473850865</v>
+        <v>0.000127459494456087</v>
       </c>
       <c r="P15" t="n">
-        <v>0.0002143757657124296</v>
+        <v>0.0001033615482582019</v>
       </c>
       <c r="Q15" t="n">
-        <v>9.005185645434368e-05</v>
+        <v>8.228326691311588e-05</v>
       </c>
       <c r="R15" t="n">
-        <v>3.426018398340754e-05</v>
+        <v>6.41017328940339e-05</v>
       </c>
       <c r="S15" t="n">
-        <v>3.459533225200791e-05</v>
+        <v>4.869978339515e-05</v>
       </c>
       <c r="T15" t="n">
-        <v>8.113702382089742e-05</v>
+        <v>3.596568775236694e-05</v>
       </c>
       <c r="U15" t="n">
-        <v>0.000165876354345007</v>
+        <v>2.579284618303003e-05</v>
       </c>
       <c r="V15" t="n">
-        <v>0.0002822926253862019</v>
+        <v>1.807950821683476e-05</v>
       </c>
       <c r="W15" t="n">
-        <v>0.000425036655101934</v>
+        <v>1.272850933107642e-05</v>
       </c>
       <c r="X15" t="n">
-        <v>0.0005896906422274964</v>
+        <v>9.647024430783654e-06</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.0007725839047007381</v>
+        <v>8.746336929508701e-06</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.000970649960607304</v>
+        <v>9.941622290764928e-06</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.001181314581200651</v>
+        <v>1.315174498464487e-05</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.001402407311923857</v>
+        <v>1.829906789988809e-05</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.001632090961638386</v>
+        <v>2.530927332956254e-05</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.001868804981682212</v>
+        <v>3.411119471934429e-05</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.002111219677566832</v>
+        <v>4.463665843182765e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>125.551724137931</v>
+        <v>124.1379310344828</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0578574132259816</v>
+        <v>0.0007016529511103959</v>
       </c>
       <c r="C16" t="n">
-        <v>0.03544701401040216</v>
+        <v>0.0006281745451752375</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02346612645575618</v>
+        <v>0.0005599349413432734</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01618697420942487</v>
+        <v>0.000496696568096779</v>
       </c>
       <c r="F16" t="n">
-        <v>0.01139265791366264</v>
+        <v>0.0004382347092153246</v>
       </c>
       <c r="G16" t="n">
-        <v>0.008077557254423292</v>
+        <v>0.0003843366619554584</v>
       </c>
       <c r="H16" t="n">
-        <v>0.005715132262502124</v>
+        <v>0.0003348009604790604</v>
       </c>
       <c r="I16" t="n">
-        <v>0.004001100981167028</v>
+        <v>0.0002894366586805799</v>
       </c>
       <c r="J16" t="n">
-        <v>0.002746692952326393</v>
+        <v>0.0002480626671581686</v>
       </c>
       <c r="K16" t="n">
-        <v>0.001828383305734625</v>
+        <v>0.0002105071396014966</v>
       </c>
       <c r="L16" t="n">
-        <v>0.001161915155949978</v>
+        <v>0.0001766069043368579</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0006878755509577278</v>
+        <v>0.0001462069371870449</v>
       </c>
       <c r="N16" t="n">
-        <v>0.0003632167566381132</v>
+        <v>0.0001191598721741751</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0001560357176841314</v>
+        <v>9.532554692492461e-05</v>
       </c>
       <c r="P16" t="n">
-        <v>4.223353603937991e-05</v>
+        <v>7.457057993302792e-05</v>
       </c>
       <c r="Q16" t="n">
-        <v>3.307427100596661e-06</v>
+        <v>5.676797709883142e-05</v>
       </c>
       <c r="R16" t="n">
-        <v>2.485017508451006e-05</v>
+        <v>4.179676520260199e-05</v>
       </c>
       <c r="S16" t="n">
-        <v>9.550563490895663e-05</v>
+        <v>2.954165018119858e-05</v>
       </c>
       <c r="T16" t="n">
-        <v>0.0002062262882394862</v>
+        <v>1.989269826884108e-05</v>
       </c>
       <c r="U16" t="n">
-        <v>0.0003497356766566583</v>
+        <v>1.274503823472766e-05</v>
       </c>
       <c r="V16" t="n">
-        <v>0.0005201327508820815</v>
+        <v>7.998583105273659e-06</v>
       </c>
       <c r="W16" t="n">
-        <v>0.0007125963800971967</v>
+        <v>5.557769898438208e-06</v>
       </c>
       <c r="X16" t="n">
-        <v>0.0009231617458717067</v>
+        <v>5.331316023941034e-06</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.001148549112288863</v>
+        <v>7.231991117228503e-06</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.001386031283479559</v>
+        <v>1.117640317844147e-05</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.001633329995075977</v>
+        <v>1.708479798122839e-05</v>
       </c>
       <c r="AB16" t="n">
-        <v>0.001888534192360341</v>
+        <v>2.488087080125146e-05</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.002150035037772931</v>
+        <v>3.449158959136806e-05</v>
       </c>
       <c r="AD16" t="n">
-        <v>0.002416473828947155</v>
+        <v>4.584702880063844e-05</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.002686699968790941</v>
+        <v>5.888021309820354e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>134.448275862069</v>
+        <v>125.8620689655172</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0534749463199354</v>
+        <v>0.0006255607442133161</v>
       </c>
       <c r="C17" t="n">
-        <v>0.03215983826900737</v>
+        <v>0.0005564048520256421</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02089072952223804</v>
+        <v>0.0004923883997333541</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01412281345893254</v>
+        <v>0.0004332771500000424</v>
       </c>
       <c r="F17" t="n">
-        <v>0.009718570872316975</v>
+        <v>0.0003788495692559145</v>
       </c>
       <c r="G17" t="n">
-        <v>0.006713153239467892</v>
+        <v>0.0003288959946285198</v>
       </c>
       <c r="H17" t="n">
-        <v>0.004603622035211921</v>
+        <v>0.0002832178655082393</v>
       </c>
       <c r="I17" t="n">
-        <v>0.003100527446813778</v>
+        <v>0.0002416270139494599</v>
       </c>
       <c r="J17" t="n">
-        <v>0.002024993062468941</v>
+        <v>0.0002039450086983704</v>
       </c>
       <c r="K17" t="n">
-        <v>0.001260399809842136</v>
+        <v>0.0001700025481614556</v>
       </c>
       <c r="L17" t="n">
-        <v>0.000727485601232968</v>
+        <v>0.000139638898093288</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0003705555341738581</v>
+        <v>0.0001127013701952004</v>
       </c>
       <c r="N17" t="n">
-        <v>0.0001493960583877994</v>
+        <v>8.904483818437734e-05</v>
       </c>
       <c r="O17" t="n">
-        <v>3.430811797125417e-05</v>
+        <v>6.853128822107854e-05</v>
       </c>
       <c r="P17" t="n">
-        <v>2.936193177870448e-06</v>
+        <v>5.102940087499785e-05</v>
       </c>
       <c r="Q17" t="n">
-        <v>3.817696155035481e-05</v>
+        <v>3.641416207409144e-05</v>
       </c>
       <c r="R17" t="n">
-        <v>0.0001267611205474831</v>
+        <v>2.456650071437532e-05</v>
       </c>
       <c r="S17" t="n">
-        <v>0.0002582683031327618</v>
+        <v>1.537295082004669e-05</v>
       </c>
       <c r="T17" t="n">
-        <v>0.0004244283171249976</v>
+        <v>8.725336332914854e-06</v>
       </c>
       <c r="U17" t="n">
-        <v>0.0006186162430447611</v>
+        <v>4.520476780570797e-06</v>
       </c>
       <c r="V17" t="n">
-        <v>0.0008354815788705275</v>
+        <v>2.659912226355228e-06</v>
       </c>
       <c r="W17" t="n">
-        <v>0.001070671827015451</v>
+        <v>3.049646042743348e-06</v>
       </c>
       <c r="X17" t="n">
-        <v>0.001320623746212899</v>
+        <v>5.599904174862567e-06</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.001582403821563924</v>
+        <v>1.022490967397206e-05</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.001853585028242351</v>
+        <v>1.684267138316049e-05</v>
       </c>
       <c r="AA17" t="n">
-        <v>0.002132150693501463</v>
+        <v>2.537478575026614e-05</v>
       </c>
       <c r="AB17" t="n">
-        <v>0.002416418822709202</v>
+        <v>3.574625082726139e-05</v>
       </c>
       <c r="AC17" t="n">
-        <v>0.002704982041295467</v>
+        <v>4.788529159174358e-05</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.00299665956789125</v>
+        <v>6.172319579573029e-05</v>
       </c>
       <c r="AE17" t="n">
-        <v>0.003290458539243181</v>
+        <v>7.719415961022516e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>143.3448275862069</v>
+        <v>127.5862068965517</v>
       </c>
       <c r="B18" t="n">
-        <v>0.04962434349069067</v>
+        <v>0.0005558200968495528</v>
       </c>
       <c r="C18" t="n">
-        <v>0.02931267927904824</v>
+        <v>0.0004908756934306268</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0186901041081548</v>
+        <v>0.000430973605721382</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01238369216857057</v>
+        <v>0.0003758828616367142</v>
       </c>
       <c r="F18" t="n">
-        <v>0.008329934268046223</v>
+        <v>0.0003253850442467029</v>
       </c>
       <c r="G18" t="n">
-        <v>0.005601716137860482</v>
+        <v>0.0002792734673000187</v>
       </c>
       <c r="H18" t="n">
-        <v>0.003717821762478368</v>
+        <v>0.0002373524147789218</v>
       </c>
       <c r="I18" t="n">
-        <v>0.002402393579032463</v>
+        <v>0.0001994364387361798</v>
       </c>
       <c r="J18" t="n">
-        <v>0.001485590110300171</v>
+        <v>0.0001653497102502677</v>
       </c>
       <c r="K18" t="n">
-        <v>0.000857079708761769</v>
+        <v>0.0001349254188536175</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0004421361889357878</v>
+        <v>0.0001080052162496542</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0001884335123093635</v>
+        <v>8.443870054398093e-05</v>
       </c>
       <c r="N18" t="n">
-        <v>5.832098669121208e-05</v>
+        <v>6.408293757984097e-05</v>
       </c>
       <c r="O18" t="n">
-        <v>2.408894873226109e-05</v>
+        <v>4.680201629364354e-05</v>
       </c>
       <c r="P18" t="n">
-        <v>6.49528979580119e-05</v>
+        <v>3.246663529700407e-05</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.0001650686932797412</v>
+        <v>2.095371815197947e-05</v>
       </c>
       <c r="R18" t="n">
-        <v>0.000312189431815229</v>
+        <v>1.21460550392676e-05</v>
       </c>
       <c r="S18" t="n">
-        <v>0.0004967344166363685</v>
+        <v>5.931968728281972e-06</v>
       </c>
       <c r="T18" t="n">
-        <v>0.0007111300780697018</v>
+        <v>2.205002945931772e-06</v>
       </c>
       <c r="U18" t="n">
-        <v>0.000949334703158657</v>
+        <v>8.63631409954625e-07</v>
       </c>
       <c r="V18" t="n">
-        <v>0.001206490044635591</v>
+        <v>1.81098594492284e-06</v>
       </c>
       <c r="W18" t="n">
-        <v>0.001478662171041614</v>
+        <v>4.954602236394399e-06</v>
       </c>
       <c r="X18" t="n">
-        <v>0.001762646148188339</v>
+        <v>1.020618190264552e-05</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.002055817073056536</v>
+        <v>1.748136967558423e-05</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.00235601523153871</v>
+        <v>2.669954458388014e-05</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.002661456692304503</v>
+        <v>3.77836241233482e-05</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.002970663077709166</v>
+        <v>5.065988048298592e-05</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.003282405944292925</v>
+        <v>6.52577679708964e-05</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.0035956624004435</v>
+        <v>8.150976085314349e-05</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.003909579444033472</v>
+        <v>9.935120088128321e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>152.2413793103448</v>
+        <v>129.3103448275862</v>
       </c>
       <c r="B19" t="n">
-        <v>0.04622061549603357</v>
+        <v>0.000492125519024551</v>
       </c>
       <c r="C19" t="n">
-        <v>0.02683204630374358</v>
+        <v>0.0004312855609566025</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01679954467565317</v>
+        <v>0.0003753929585381142</v>
       </c>
       <c r="E19" t="n">
-        <v>0.01091189396742268</v>
+        <v>0.0003242199381415125</v>
       </c>
       <c r="F19" t="n">
-        <v>0.007174758423416096</v>
+        <v>0.0002775511355167514</v>
       </c>
       <c r="G19" t="n">
-        <v>0.004696057653599798</v>
+        <v>0.00023518277975363</v>
       </c>
       <c r="H19" t="n">
-        <v>0.003014641940527609</v>
+        <v>0.0001969219406824689</v>
       </c>
       <c r="I19" t="n">
-        <v>0.001867159711306765</v>
+        <v>0.0001625858340126479</v>
       </c>
       <c r="J19" t="n">
-        <v>0.001092055280354705</v>
+        <v>0.0001320011790895076</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0005847472266276857</v>
+        <v>0.0001050036046648005</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0002746478505008818</v>
+        <v>8.143709853277872e-05</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0001124983725434393</v>
+        <v>6.115349729052219e-05</v>
       </c>
       <c r="N19" t="n">
-        <v>6.29771420079127e-05</v>
+        <v>4.401201284281417e-05</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0001001793235239975</v>
+        <v>2.987879259488577e-05</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0002047434729606287</v>
+        <v>1.862651056450679e-05</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.0003619644022106923</v>
+        <v>1.013398690309079e-05</v>
       </c>
       <c r="R19" t="n">
-        <v>0.0005605187540027292</v>
+        <v>4.285833546504182e-06</v>
       </c>
       <c r="S19" t="n">
-        <v>0.000791583367040699</v>
+        <v>9.721239236793285e-07</v>
       </c>
       <c r="T19" t="n">
-        <v>0.00104821241172545</v>
+        <v>8.808483744096325e-08</v>
       </c>
       <c r="U19" t="n">
-        <v>0.001324889127176691</v>
+        <v>1.533808799520316e-06</v>
       </c>
       <c r="V19" t="n">
-        <v>0.001617197880545894</v>
+        <v>5.213985252684922e-06</v>
       </c>
       <c r="W19" t="n">
-        <v>0.001921580715025651</v>
+        <v>1.103764924906297e-05</v>
       </c>
       <c r="X19" t="n">
-        <v>0.002235154230319632</v>
+        <v>1.891794627662177e-05</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.0025555702028321</v>
+        <v>2.877191203695011e-05</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.00288090835346377</v>
+        <v>4.052026607798573e-05</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.003209593039095637</v>
+        <v>5.408721827655351e-05</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.003540327951140645</v>
+        <v>6.940028724819357e-05</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.003872044509652439</v>
+        <v>8.639012983682237e-05</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.00420386077398471</v>
+        <v>0.0001049903809050995</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.00453504850049564</v>
+        <v>0.0001251375027083807</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>161.1379310344828</v>
+        <v>131.0344827586207</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0431958487250765</v>
+        <v>0.0004341884268890952</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02465962905335673</v>
+        <v>0.0003773496653375326</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01516798056516758</v>
+        <v>0.0003253653928549538</v>
       </c>
       <c r="E20" t="n">
-        <v>0.009662064197977702</v>
+        <v>0.0002780109695248495</v>
       </c>
       <c r="F20" t="n">
-        <v>0.006212348222111394</v>
+        <v>0.0002350740217822839</v>
       </c>
       <c r="G20" t="n">
-        <v>0.003959374324257306</v>
+        <v>0.0001963536346655396</v>
       </c>
       <c r="H20" t="n">
-        <v>0.00246059108360547</v>
+        <v>0.0001616596069227429</v>
       </c>
       <c r="I20" t="n">
-        <v>0.001464195399195844</v>
+        <v>0.0001308117633214472</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0008162598266898082</v>
+        <v>0.0001036393190851305</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0004174832671796563</v>
+        <v>7.998029189147944e-05</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0002010698649606147</v>
+        <v>5.968095732042786e-05</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0001205656678098358</v>
+        <v>4.259534404317925e-05</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0001427750485670393</v>
+        <v>2.85847654022572e-05</v>
       </c>
       <c r="O20" t="n">
-        <v>0.000243438045943401</v>
+        <v>1.751738435290778e-05</v>
       </c>
       <c r="P20" t="n">
-        <v>0.000404488253789689</v>
+        <v>9.267809022072246e-06</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.0006122555721796648</v>
+        <v>3.716716397098817e-06</v>
       </c>
       <c r="R20" t="n">
-        <v>0.0008562549079346607</v>
+        <v>7.505018855082618e-07</v>
       </c>
       <c r="S20" t="n">
-        <v>0.001128349868060972</v>
+        <v>2.609526927788736e-07</v>
       </c>
       <c r="T20" t="n">
-        <v>0.001422163083726333</v>
+        <v>2.144943149839509e-06</v>
       </c>
       <c r="U20" t="n">
-        <v>0.001732652668272615</v>
+        <v>6.304150288097315e-06</v>
       </c>
       <c r="V20" t="n">
-        <v>0.002055802974451909</v>
+        <v>1.264478810950163e-05</v>
       </c>
       <c r="W20" t="n">
-        <v>0.002388395480036532</v>
+        <v>2.107735913407925e-05</v>
       </c>
       <c r="X20" t="n">
-        <v>0.002727836799143083</v>
+        <v>3.151642192923905e-05</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.003072028041115655</v>
+        <v>4.388037343531445e-05</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.003419264509326032</v>
+        <v>5.809124500144172e-05</v>
       </c>
       <c r="AA20" t="n">
-        <v>0.003768157941463688</v>
+        <v>7.407451113628862e-05</v>
       </c>
       <c r="AB20" t="n">
-        <v>0.004117575688581067</v>
+        <v>9.175891006000484e-05</v>
       </c>
       <c r="AC20" t="n">
-        <v>0.004466592755765172</v>
+        <v>0.0001110762752181728</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.004814453702412133</v>
+        <v>0.0001319613769862709</v>
       </c>
       <c r="AE20" t="n">
-        <v>0.00516054216762353</v>
+        <v>0.0001543517738545107</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>170.0344827586207</v>
+        <v>132.7586206896552</v>
       </c>
       <c r="B21" t="n">
-        <v>0.04049510715483079</v>
+        <v>0.0003817360384409591</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0227485838983801</v>
+        <v>0.000328798843057889</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01375459382395367</v>
+        <v>0.0002806252960694786</v>
       </c>
       <c r="E21" t="n">
-        <v>0.00859810908300563</v>
+        <v>0.0002369938284866984</v>
       </c>
       <c r="F21" t="n">
-        <v>0.005410442583877972</v>
+        <v>0.0001976949973191018</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00336259467310569</v>
+        <v>0.0001625306859701291</v>
       </c>
       <c r="H21" t="n">
-        <v>0.002029304416156872</v>
+        <v>0.0001313133669138391</v>
       </c>
       <c r="I21" t="n">
-        <v>0.00116946842423257</v>
+        <v>0.0001038654210484786</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0006362068968660686</v>
+        <v>8.00185086938255e-05</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0003350854516861861</v>
+        <v>5.961298770610906e-05</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0002027957677868853</v>
+        <v>4.24973746338481e-05</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0001954588551790807</v>
+        <v>2.85278452378917e-05</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0002818276348711689</v>
+        <v>1.756777105501339e-05</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0004391474328739665</v>
+        <v>9.487289001913574e-06</v>
       </c>
       <c r="P21" t="n">
-        <v>0.0006505353372834661</v>
+        <v>4.162901300201073e-06</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.0009032659655491686</v>
+        <v>1.477103256656485e-06</v>
       </c>
       <c r="R21" t="n">
-        <v>0.001187618382497783</v>
+        <v>1.318036660372047e-06</v>
       </c>
       <c r="S21" t="n">
-        <v>0.001496081542724392</v>
+        <v>3.579166762303665e-06</v>
       </c>
       <c r="T21" t="n">
-        <v>0.001822795144985676</v>
+        <v>8.158980985883444e-06</v>
       </c>
       <c r="U21" t="n">
-        <v>0.002163148805762616</v>
+        <v>1.496070768216916e-05</v>
       </c>
       <c r="V21" t="n">
-        <v>0.00251348997943778</v>
+        <v>2.389205339127581e-05</v>
       </c>
       <c r="W21" t="n">
-        <v>0.002870907991416237</v>
+        <v>3.486495720575998e-05</v>
       </c>
       <c r="X21" t="n">
-        <v>0.003233072246828568</v>
+        <v>4.779536095229193e-05</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.0035981095881438</v>
+        <v>6.260299401725969e-05</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.003964510332726916</v>
+        <v>7.921117174070094e-05</v>
       </c>
       <c r="AA21" t="n">
-        <v>0.004331055583711489</v>
+        <v>9.754660639250468e-05</v>
       </c>
       <c r="AB21" t="n">
-        <v>0.004696760500235329</v>
+        <v>0.0001175392298260302</v>
       </c>
       <c r="AC21" t="n">
-        <v>0.00506082966537195</v>
+        <v>0.00013912202697805</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.005422621712303639</v>
+        <v>0.0001622308794509332</v>
       </c>
       <c r="AE21" t="n">
-        <v>0.005781621098192682</v>
+        <v>0.0001868044184739299</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>178.9310344827586</v>
+        <v>134.4827586206897</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0380734663362695</v>
+        <v>0.0003345103530860421</v>
       </c>
       <c r="C22" t="n">
-        <v>0.02106086037789633</v>
+        <v>0.0002853785460403979</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01252639428389491</v>
+        <v>0.0002409215079526239</v>
       </c>
       <c r="E22" t="n">
-        <v>0.007690979875903304</v>
+        <v>0.0002009206798606118</v>
       </c>
       <c r="F22" t="n">
-        <v>0.004743176191589787</v>
+        <v>0.0001651694910449557</v>
       </c>
       <c r="G22" t="n">
-        <v>0.002882493766164122</v>
+        <v>0.0001334725674262664</v>
       </c>
       <c r="H22" t="n">
-        <v>0.001699791591394935</v>
+        <v>0.00010564500167977</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0009639097883930495</v>
+        <v>8.151167950926242e-05</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0005345007690028825</v>
+        <v>6.090665708977696e-05</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0003216307528733827</v>
+        <v>4.367258519095511e-05</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0002652102428163105</v>
+        <v>2.966017593937665e-05</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0003237326600231471</v>
+        <v>1.872770857465882e-05</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0004677433726103592</v>
+        <v>1.074057090743931e-05</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0006758704172758967</v>
+        <v>5.570833502326495e-06</v>
       </c>
       <c r="P22" t="n">
-        <v>0.0009323165680197868</v>
+        <v>3.09685389024205e-06</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.001225222021747778</v>
+        <v>3.202908366292184e-06</v>
       </c>
       <c r="R22" t="n">
-        <v>0.001545565184960706</v>
+        <v>5.778849154706197e-06</v>
       </c>
       <c r="S22" t="n">
-        <v>0.001886406698686961</v>
+        <v>1.071978492460424e-05</v>
       </c>
       <c r="T22" t="n">
-        <v>0.002242358475431672</v>
+        <v>1.79257828220037e-05</v>
       </c>
       <c r="U22" t="n">
-        <v>0.002609203819046198</v>
+        <v>2.730159034683607e-05</v>
       </c>
       <c r="V22" t="n">
-        <v>0.002983621155274229</v>
+        <v>3.875637555080997e-05</v>
       </c>
       <c r="W22" t="n">
-        <v>0.003362980164877574</v>
+        <v>5.220348416476107e-05</v>
       </c>
       <c r="X22" t="n">
-        <v>0.003745189368927664</v>
+        <v>6.756021238366768e-05</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.004128580835133978</v>
+        <v>8.474759414599691e-05</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.00451182203437354</v>
+        <v>0.0001036902018418294</v>
       </c>
       <c r="AA22" t="n">
-        <v>0.004893847802789722</v>
+        <v>0.0001243159594730598</v>
       </c>
       <c r="AB22" t="n">
-        <v>0.005273807362109911</v>
+        <v>0.0001465559673694083</v>
       </c>
       <c r="AC22" t="n">
-        <v>0.005651022735275295</v>
+        <v>0.0001703443376371021</v>
       </c>
       <c r="AD22" t="n">
-        <v>0.006024955867785692</v>
+        <v>0.0001956180395834997</v>
       </c>
       <c r="AE22" t="n">
-        <v>0.006395182458383606</v>
+        <v>0.0002223167544213358</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>187.8275862068965</v>
+        <v>136.2068965517241</v>
       </c>
       <c r="B23" t="n">
-        <v>0.03589382931083902</v>
+        <v>0.000292267207788634</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01956524261587779</v>
+        <v>0.0002468479072286683</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01145645000902559</v>
+        <v>0.0002060163955076102</v>
       </c>
       <c r="E23" t="n">
-        <v>0.006917061052339407</v>
+        <v>0.0001695570645968168</v>
       </c>
       <c r="F23" t="n">
-        <v>0.004189600967642535</v>
+        <v>0.0001372661594787092</v>
       </c>
       <c r="G23" t="n">
-        <v>0.002500328959859837</v>
+        <v>0.0001089509944082133</v>
       </c>
       <c r="H23" t="n">
-        <v>0.00145517170354542</v>
+        <v>8.442923033646273e-05</v>
       </c>
       <c r="I23" t="n">
-        <v>0.0008322359315114145</v>
+        <v>6.352820798492596e-05</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0004972464188066907</v>
+        <v>4.608433162090181e-05</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0003644442360941731</v>
+        <v>3.194249908415372e-05</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0003767201668518144</v>
+        <v>2.095557405712068e-05</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0004947605838431155</v>
+        <v>1.298389696468007e-05</v>
       </c>
       <c r="N23" t="n">
-        <v>0.0006907652337307167</v>
+        <v>7.894831239834068e-06</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0009446366118582587</v>
+        <v>5.562342004207401e-06</v>
       </c>
       <c r="P23" t="n">
-        <v>0.001241576917983942</v>
+        <v>5.866604491276519e-06</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.001570522221085135</v>
+        <v>8.693639789936995e-06</v>
       </c>
       <c r="R23" t="n">
-        <v>0.001923093241980681</v>
+        <v>1.393497570956693e-05</v>
       </c>
       <c r="S23" t="n">
-        <v>0.002292875145174272</v>
+        <v>2.148733076830195e-05</v>
       </c>
       <c r="T23" t="n">
-        <v>0.002674912673374761</v>
+        <v>3.125231948638514e-05</v>
       </c>
       <c r="U23" t="n">
-        <v>0.003065349644429381</v>
+        <v>4.313617732843719e-05</v>
       </c>
       <c r="V23" t="n">
-        <v>0.003461167293904062</v>
+        <v>5.70495037843522e-05</v>
       </c>
       <c r="W23" t="n">
-        <v>0.003859991581119806</v>
+        <v>7.29070222101549e-05</v>
       </c>
       <c r="X23" t="n">
-        <v>0.004259949425290534</v>
+        <v>9.062735516873668e-05</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.004659560186343047</v>
+        <v>0.0001101328141178927</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.005057652881626286</v>
+        <v>0.0001313492023900568</v>
       </c>
       <c r="AA23" t="n">
-        <v>0.005453302429383217</v>
+        <v>0.0001542056304961511</v>
       </c>
       <c r="AB23" t="n">
-        <v>0.005845780118535177</v>
+        <v>0.0001786343428658512</v>
       </c>
       <c r="AC23" t="n">
-        <v>0.006234514825810564</v>
+        <v>0.0002045705552088077</v>
       </c>
       <c r="AD23" t="n">
-        <v>0.00661906242920793</v>
+        <v>0.0002319523017474164</v>
       </c>
       <c r="AE23" t="n">
-        <v>0.006999081526927051</v>
+        <v>0.000260720291631522</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>196.7241379310345</v>
+        <v>137.9310344827586</v>
       </c>
       <c r="B24" t="n">
-        <v>0.03392529315435848</v>
+        <v>0.0002547754032484008</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01823589179680067</v>
+        <v>0.0002129788755576682</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01052257542583979</v>
+        <v>0.0001756849965877764</v>
       </c>
       <c r="E24" t="n">
-        <v>0.00625697909954939</v>
+        <v>0.0001426810518851572</v>
       </c>
       <c r="F24" t="n">
-        <v>0.00373259631969143</v>
+        <v>0.0001137660472298319</v>
       </c>
       <c r="G24" t="n">
-        <v>0.002200836819157334</v>
+        <v>8.874993262663419e-05</v>
       </c>
       <c r="H24" t="n">
-        <v>0.001281745283554897</v>
+        <v>6.745288691274777e-05</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0007620865298666498</v>
+        <v>4.970465751490788e-05</v>
       </c>
       <c r="J24" t="n">
-        <v>0.000513245568414346</v>
+        <v>3.534395044828421e-05</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0004533471115067874</v>
+        <v>2.421786614394052e-05</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0005280494280076071</v>
+        <v>1.618137713100225e-05</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0007000720464029055</v>
+        <v>1.109684399016272e-05</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0009431463494098544</v>
+        <v>8.833566342718912e-06</v>
       </c>
       <c r="O24" t="n">
-        <v>0.001238353193021229</v>
+        <v>9.267365949424544e-06</v>
       </c>
       <c r="P24" t="n">
-        <v>0.001571817726240864</v>
+        <v>1.228019927020368e-05</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.001933210161497363</v>
+        <v>1.775979708345755e-05</v>
       </c>
       <c r="R24" t="n">
-        <v>0.002314743088409563</v>
+        <v>2.559932898543561e-05</v>
       </c>
       <c r="S24" t="n">
-        <v>0.002710484516948179</v>
+        <v>3.569709078903996e-05</v>
       </c>
       <c r="T24" t="n">
-        <v>0.003115877249035526</v>
+        <v>4.795621302012691e-05</v>
       </c>
       <c r="U24" t="n">
-        <v>0.003527396353854477</v>
+        <v>6.228438886997474e-05</v>
       </c>
       <c r="V24" t="n">
-        <v>0.003942301055490652</v>
+        <v>7.859362010727029e-05</v>
       </c>
       <c r="W24" t="n">
-        <v>0.004358452387214309</v>
+        <v>9.679997958344109e-05</v>
       </c>
       <c r="X24" t="n">
-        <v>0.004774177433490364</v>
+        <v>0.0001168233890827808</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.005188167075401665</v>
+        <v>0.000138587411375385</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.005599398160474387</v>
+        <v>0.0001620190554271008</v>
       </c>
       <c r="AA24" t="n">
-        <v>0.006007073699615352</v>
+        <v>0.0001870485938078362</v>
       </c>
       <c r="AB24" t="n">
-        <v>0.006410576520030732</v>
+        <v>0.000213609391418937</v>
       </c>
       <c r="AC24" t="n">
-        <v>0.006809433065878398</v>
+        <v>0.0002416377447318228</v>
       </c>
       <c r="AD24" t="n">
-        <v>0.007203284924188887</v>
+        <v>0.0002710727307955693</v>
       </c>
       <c r="AE24" t="n">
-        <v>0.007591866282989233</v>
+        <v>0.0003018560653304215</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>205.6206896551724</v>
+        <v>139.6551724137931</v>
       </c>
       <c r="B25" t="n">
-        <v>0.03214191002723818</v>
+        <v>0.0002218158941737554</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01705124607012268</v>
+        <v>0.0001835554144317298</v>
       </c>
       <c r="D25" t="n">
-        <v>0.009706344816799963</v>
+        <v>0.0001497142264424019</v>
       </c>
       <c r="E25" t="n">
-        <v>0.005694709458372572</v>
+        <v>0.0001200824536355938</v>
       </c>
       <c r="F25" t="n">
-        <v>0.003358054301404477</v>
+        <v>9.446180928382844e-05</v>
       </c>
       <c r="G25" t="n">
-        <v>0.001971484874404643</v>
+        <v>7.26648280926521e-05</v>
       </c>
       <c r="H25" t="n">
-        <v>0.001168303589682745</v>
+        <v>5.451415786988541e-05</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0007433841024016865</v>
+        <v>3.984190585196095e-05</v>
       </c>
       <c r="J25" t="n">
-        <v>0.0005734007498392232</v>
+        <v>2.84890348196047e-05</v>
       </c>
       <c r="K25" t="n">
-        <v>0.0005801004222226147</v>
+        <v>2.030480462639868e-05</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0007117181963338887</v>
+        <v>1.514625519953205e-05</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0009328638167220362</v>
+        <v>1.287772745951394e-05</v>
       </c>
       <c r="N25" t="n">
-        <v>0.001218690673793989</v>
+        <v>1.337041895046862e-05</v>
       </c>
       <c r="O25" t="n">
-        <v>0.00155137226964302</v>
+        <v>1.650197128026276e-05</v>
       </c>
       <c r="P25" t="n">
-        <v>0.001917888572599809</v>
+        <v>2.215608674431199e-05</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.002308589008130873</v>
+        <v>3.022217175255699e-05</v>
       </c>
       <c r="R25" t="n">
-        <v>0.002716233190658949</v>
+        <v>4.059500489908611e-05</v>
       </c>
       <c r="S25" t="n">
-        <v>0.00313533496069929</v>
+        <v>5.317442771118779e-05</v>
       </c>
       <c r="T25" t="n">
-        <v>0.003561704325992975</v>
+        <v>6.786505629179086e-05</v>
       </c>
       <c r="U25" t="n">
-        <v>0.003992121662897559</v>
+        <v>8.457601222858106e-05</v>
       </c>
       <c r="V25" t="n">
-        <v>0.004424102194736103</v>
+        <v>0.0001032206712865547</v>
       </c>
       <c r="W25" t="n">
-        <v>0.004855723257376315</v>
+        <v>0.0001237164285301104</v>
       </c>
       <c r="X25" t="n">
-        <v>0.005285495971233969</v>
+        <v>0.0001459844786375401</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.005712268796399793</v>
+        <v>0.0001699496102762892</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.006135154292687845</v>
+        <v>0.0001955400135027969</v>
       </c>
       <c r="AA25" t="n">
-        <v>0.006553472977921609</v>
+        <v>0.0002226870992372292</v>
       </c>
       <c r="AB25" t="n">
-        <v>0.006966709926882133</v>
+        <v>0.0002513253299418278</v>
       </c>
       <c r="AC25" t="n">
-        <v>0.007374480961555077</v>
+        <v>0.0002813920607028066</v>
       </c>
       <c r="AD25" t="n">
-        <v>0.007776506129764546</v>
+        <v>0.0003128273899803303</v>
       </c>
       <c r="AE25" t="n">
-        <v>0.008172588770036061</v>
+        <v>0.0003455740193501553</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>214.5172413793103</v>
+        <v>141.3793103448276</v>
       </c>
       <c r="B26" t="n">
-        <v>0.03052173533201142</v>
+        <v>0.0001931810382853341</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01599317951872437</v>
+        <v>0.0001583727583895736</v>
       </c>
       <c r="D26" t="n">
-        <v>0.008992340854852683</v>
+        <v>0.0001279021419151539</v>
       </c>
       <c r="E26" t="n">
-        <v>0.005216898259207011</v>
+        <v>0.0001015620960852011</v>
       </c>
       <c r="F26" t="n">
-        <v>0.003054262355280908</v>
+        <v>7.915698989633894e-05</v>
       </c>
       <c r="G26" t="n">
-        <v>0.001801906140501034</v>
+        <v>6.050189318061109e-05</v>
       </c>
       <c r="H26" t="n">
-        <v>0.001105607744804182</v>
+        <v>4.542187521767968e-05</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0007678520873142082</v>
+        <v>3.375135751920102e-05</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0006702677260393938</v>
+        <v>2.533351595754683e-05</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0007379880292090004</v>
+        <v>2.001972789835932e-05</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0009216533168926324</v>
+        <v>1.766906042896746e-05</v>
       </c>
       <c r="M26" t="n">
-        <v>0.001187635147640902</v>
+        <v>1.814779615906849e-05</v>
       </c>
       <c r="N26" t="n">
-        <v>0.001512410582340514</v>
+        <v>2.132899341236777e-05</v>
       </c>
       <c r="O26" t="n">
-        <v>0.001879168981427516</v>
+        <v>2.70920779329633e-05</v>
       </c>
       <c r="P26" t="n">
-        <v>0.002275684168829752</v>
+        <v>3.532246350275106e-05</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.002692935682464429</v>
+        <v>4.591119910981981e-05</v>
       </c>
       <c r="R26" t="n">
-        <v>0.003124190115958295</v>
+        <v>5.875464052600279e-05</v>
       </c>
       <c r="S26" t="n">
-        <v>0.003564374115986285</v>
+        <v>7.375414434752104e-05</v>
       </c>
       <c r="T26" t="n">
-        <v>0.004009637392201751</v>
+        <v>9.081578272824453e-05</v>
       </c>
       <c r="U26" t="n">
-        <v>0.004457042518822531</v>
+        <v>0.0001098500771933742</v>
       </c>
       <c r="V26" t="n">
-        <v>0.004904341146464999</v>
+        <v>0.0001307717500633873</v>
       </c>
       <c r="W26" t="n">
-        <v>0.005349810217651433</v>
+        <v>0.0001534994921465207</v>
       </c>
       <c r="X26" t="n">
-        <v>0.005792130552405056</v>
+        <v>0.0001779557454737662</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.006230295805472206</v>
+        <v>0.0002040664999550541</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.006663543491659716</v>
+        <v>0.0002317611029298023</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.007091302244082803</v>
+        <v>0.0002609720806709897</v>
       </c>
       <c r="AB26" t="n">
-        <v>0.007513151147118601</v>
+        <v>0.0002916349709794478</v>
       </c>
       <c r="AC26" t="n">
-        <v>0.007928788142935574</v>
+        <v>0.0003236881660757102</v>
       </c>
       <c r="AD26" t="n">
-        <v>0.00833800532016178</v>
+        <v>0.0003570727650609339</v>
       </c>
       <c r="AE26" t="n">
-        <v>0.008740669467249159</v>
+        <v>0.0003917324352767055</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>223.4137931034483</v>
+        <v>143.1034482758621</v>
       </c>
       <c r="B27" t="n">
-        <v>0.02904608782494592</v>
+        <v>0.0001686738991883136</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01504635163315416</v>
+        <v>0.0001372367231367245</v>
       </c>
       <c r="D27" t="n">
-        <v>0.008367575422318909</v>
+        <v>0.0001100572585163838</v>
       </c>
       <c r="E27" t="n">
-        <v>0.004812341081783721</v>
+        <v>8.693114379344606e-05</v>
       </c>
       <c r="F27" t="n">
-        <v>0.002811430161983924</v>
+        <v>6.766535339736841e-05</v>
       </c>
       <c r="G27" t="n">
-        <v>0.001683466655952866</v>
+        <v>5.207744413036729e-05</v>
       </c>
       <c r="H27" t="n">
-        <v>0.001085991255824624</v>
+        <v>3.999486060667324e-05</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0008286478292958163</v>
+        <v>3.125429438683334e-05</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0007977153054810533</v>
+        <v>2.570109201834092e-05</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0009215002648576794</v>
+        <v>2.318870767762306e-05</v>
       </c>
       <c r="L27" t="n">
-        <v>0.001152893312989452</v>
+        <v>2.357819653752283e-05</v>
       </c>
       <c r="M27" t="n">
-        <v>0.001459912028717266</v>
+        <v>2.673774536599947e-05</v>
       </c>
       <c r="N27" t="n">
-        <v>0.001820268583392734</v>
+        <v>3.254223720125988e-05</v>
       </c>
       <c r="O27" t="n">
-        <v>0.002218099127091645</v>
+        <v>4.08728472513378e-05</v>
       </c>
       <c r="P27" t="n">
-        <v>0.002641916564535611</v>
+        <v>5.161666743650318e-05</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.003083286474645921</v>
+        <v>6.466635723454302e-05</v>
       </c>
       <c r="R27" t="n">
-        <v>0.003535946519782514</v>
+        <v>7.991981870561748e-05</v>
       </c>
       <c r="S27" t="n">
-        <v>0.003995206564097404</v>
+        <v>9.727989376729822e-05</v>
       </c>
       <c r="T27" t="n">
-        <v>0.004457531396522742</v>
+        <v>0.0001166540819649192</v>
       </c>
       <c r="U27" t="n">
-        <v>0.004920245116419557</v>
+        <v>0.0001379542771390767</v>
       </c>
       <c r="V27" t="n">
-        <v>0.005381318305921578</v>
+        <v>0.0001610965215331269</v>
       </c>
       <c r="W27" t="n">
-        <v>0.005839212599490303</v>
+        <v>0.0001860007760108929</v>
       </c>
       <c r="X27" t="n">
-        <v>0.006292765718190914</v>
+        <v>0.0002125907051695517</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.006741105462308498</v>
+        <v>0.0002407934762363776</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.007183584709848331</v>
+        <v>0.0002705395707319705</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.00761973183990219</v>
+        <v>0.0003017626079675612</v>
       </c>
       <c r="AB27" t="n">
-        <v>0.008049212609228078</v>
+        <v>0.0003343991795210942</v>
       </c>
       <c r="AC27" t="n">
-        <v>0.00847180061953407</v>
+        <v>0.0003683886939067223</v>
       </c>
       <c r="AD27" t="n">
-        <v>0.008887354288214095</v>
+        <v>0.0004036732307159903</v>
       </c>
       <c r="AE27" t="n">
-        <v>0.009295798784222244</v>
+        <v>0.0004401974035668015</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>232.3103448275862</v>
+        <v>144.8275862068965</v>
       </c>
       <c r="B28" t="n">
-        <v>0.02769896827311094</v>
+        <v>0.0001481075987042119</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01419769874032511</v>
+        <v>0.0001199630645740656</v>
       </c>
       <c r="D28" t="n">
-        <v>0.007821038403130044</v>
+        <v>9.599791603566119e-05</v>
       </c>
       <c r="E28" t="n">
-        <v>0.004471578049169251</v>
+        <v>7.601047172883155e-05</v>
       </c>
       <c r="F28" t="n">
-        <v>0.00262132301191692</v>
+        <v>5.981026264524541e-05</v>
       </c>
       <c r="G28" t="n">
-        <v>0.001608931148171538</v>
+        <v>4.72172857643764e-05</v>
       </c>
       <c r="H28" t="n">
-        <v>0.001103053377997878</v>
+        <v>3.806131620698177e-05</v>
       </c>
       <c r="I28" t="n">
-        <v>0.0009200800241270123</v>
+        <v>3.218127261389381e-05</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0009506639556090188</v>
+        <v>2.942463100008713e-05</v>
       </c>
       <c r="K28" t="n">
-        <v>0.001126091330855633</v>
+        <v>2.964688281389766e-05</v>
       </c>
       <c r="L28" t="n">
-        <v>0.00140136258586727</v>
+        <v>3.271103335734652e-05</v>
       </c>
       <c r="M28" t="n">
-        <v>0.001746036517964182</v>
+        <v>3.848713710197443e-05</v>
       </c>
       <c r="N28" t="n">
-        <v>0.00213898035991817</v>
+        <v>4.685186677166595e-05</v>
       </c>
       <c r="O28" t="n">
-        <v>0.002565214693255884</v>
+        <v>5.768811336428831e-05</v>
       </c>
       <c r="P28" t="n">
-        <v>0.003013942102653959</v>
+        <v>7.0884614552228e-05</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.003477274498840823</v>
+        <v>8.633560914183255e-05</v>
       </c>
       <c r="R28" t="n">
-        <v>0.003949388285743742</v>
+        <v>0.0001039405154863761</v>
       </c>
       <c r="S28" t="n">
-        <v>0.004425949930865212</v>
+        <v>0.000123603631939967</v>
       </c>
       <c r="T28" t="n">
-        <v>0.004903717172264022</v>
+        <v>0.000145233857612582</v>
       </c>
       <c r="U28" t="n">
-        <v>0.005380257067912781</v>
+        <v>0.0001687444318419835</v>
       </c>
       <c r="V28" t="n">
-        <v>0.005853743429025058</v>
+        <v>0.0001940526909382034</v>
       </c>
       <c r="W28" t="n">
-        <v>0.006322809204819037</v>
+        <v>0.0002210798408825655</v>
       </c>
       <c r="X28" t="n">
-        <v>0.006786437545376065</v>
+        <v>0.0002497507447768948</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.007243880498522932</v>
+        <v>0.0002799937239416262</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.00769459771787826</v>
+        <v>0.0003117403716546156</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.008138209839542604</v>
+        <v>0.0003449253786065835</v>
       </c>
       <c r="AB28" t="n">
-        <v>0.008574462730710341</v>
+        <v>0.000379486369225758</v>
       </c>
       <c r="AC28" t="n">
-        <v>0.009003199877603608</v>
+        <v>0.0004153637480935762</v>
       </c>
       <c r="AD28" t="n">
-        <v>0.009424340923059112</v>
+        <v>0.0004525005557362957</v>
       </c>
       <c r="AE28" t="n">
-        <v>0.009837864889531967</v>
+        <v>0.000490842333134822</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>241.2068965517241</v>
+        <v>146.551724137931</v>
       </c>
       <c r="B29" t="n">
-        <v>0.02646659815957138</v>
+        <v>0.0001313047146585394</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01343603249932168</v>
+        <v>0.0001063768828535726</v>
       </c>
       <c r="D29" t="n">
-        <v>0.007343342698477757</v>
+        <v>8.555168875967999e-05</v>
       </c>
       <c r="E29" t="n">
-        <v>0.004186576170363534</v>
+        <v>6.863008154595769e-05</v>
       </c>
       <c r="F29" t="n">
-        <v>0.00247697488887601</v>
+        <v>5.542410126241052e-05</v>
       </c>
       <c r="G29" t="n">
-        <v>0.001572201980515851</v>
+        <v>4.575613958453019e-05</v>
       </c>
       <c r="H29" t="n">
-        <v>0.001151420197062353</v>
+        <v>3.945825857092831e-05</v>
       </c>
       <c r="I29" t="n">
-        <v>0.001037389009330167</v>
+        <v>3.637156218392826e-05</v>
       </c>
       <c r="J29" t="n">
-        <v>0.001124882953623709</v>
+        <v>3.634561586101056e-05</v>
       </c>
       <c r="K29" t="n">
-        <v>0.00134799138981029</v>
+        <v>3.923790990152589e-05</v>
       </c>
       <c r="L29" t="n">
-        <v>0.001663696854247558</v>
+        <v>4.491336285571255e-05</v>
       </c>
       <c r="M29" t="n">
-        <v>0.002043004189765523</v>
+        <v>5.3243861478959e-05</v>
       </c>
       <c r="N29" t="n">
-        <v>0.002465863086538166</v>
+        <v>6.41078341484119e-05</v>
       </c>
       <c r="O29" t="n">
-        <v>0.002918122062091092</v>
+        <v>7.738985493737373e-05</v>
       </c>
       <c r="P29" t="n">
-        <v>0.00338962867001149</v>
+        <v>9.29802758088957e-05</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.003873005246671369</v>
+        <v>0.0001107748846281298</v>
       </c>
       <c r="R29" t="n">
-        <v>0.004362837731459339</v>
+        <v>0.0001306745869059314</v>
       </c>
       <c r="S29" t="n">
-        <v>0.004855125169739667</v>
+        <v>0.0001525851093774275</v>
       </c>
       <c r="T29" t="n">
-        <v>0.005346898285944196</v>
+        <v>0.0001764167236907252</v>
       </c>
       <c r="U29" t="n">
-        <v>0.005835950360266927</v>
+        <v>0.0002020839886351615</v>
       </c>
       <c r="V29" t="n">
-        <v>0.006320644287787811</v>
+        <v>0.0002295055094774767</v>
       </c>
       <c r="W29" t="n">
-        <v>0.006799772289533119</v>
+        <v>0.0002586037130992778</v>
       </c>
       <c r="X29" t="n">
-        <v>0.007272452623008473</v>
+        <v>0.0002893046377421824</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.007738052683306635</v>
+        <v>0.0003215377362691613</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.008196131181980976</v>
+        <v>0.0003552356919427298</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.008646394285380209</v>
+        <v>0.0003903342458044421</v>
       </c>
       <c r="AB29" t="n">
-        <v>0.009088662080081869</v>
+        <v>0.000426772034815738</v>
       </c>
       <c r="AC29" t="n">
-        <v>0.00952284275481648</v>
+        <v>0.0004644904399892345</v>
       </c>
       <c r="AD29" t="n">
-        <v>0.009948912600798469</v>
+        <v>0.0005034334438016963</v>
       </c>
       <c r="AE29" t="n">
-        <v>0.01036690043571669</v>
+        <v>0.0005435474962372832</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>250.1034482758621</v>
+        <v>148.2758620689655</v>
       </c>
       <c r="B30" t="n">
-        <v>0.02533705032107018</v>
+        <v>0.000118096720484562</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01275172005784456</v>
+        <v>9.631206785336286e-05</v>
       </c>
       <c r="D30" t="n">
-        <v>0.006926442407651354</v>
+        <v>7.855483671910185e-05</v>
       </c>
       <c r="E30" t="n">
-        <v>0.003950477857068362</v>
+        <v>6.462855850726252e-05</v>
       </c>
       <c r="F30" t="n">
-        <v>0.002372461879331471</v>
+        <v>5.434773613780825e-05</v>
       </c>
       <c r="G30" t="n">
-        <v>0.001568113448686995</v>
+        <v>4.753711176333168e-05</v>
       </c>
       <c r="H30" t="n">
-        <v>0.001226556764360071</v>
+        <v>4.403099202359213e-05</v>
       </c>
       <c r="I30" t="n">
-        <v>0.001176574352703834</v>
+        <v>4.367262560772729e-05</v>
       </c>
       <c r="J30" t="n">
-        <v>0.001316831519103316</v>
+        <v>4.631362844951225e-05</v>
       </c>
       <c r="K30" t="n">
-        <v>0.001584059684669858</v>
+        <v>5.181345235398755e-05</v>
       </c>
       <c r="L30" t="n">
-        <v>0.001937106970248222</v>
+        <v>6.003889327328138e-05</v>
       </c>
       <c r="M30" t="n">
-        <v>0.002348337563830463</v>
+        <v>7.08636358224639e-05</v>
       </c>
       <c r="N30" t="n">
-        <v>0.002798717551236263</v>
+        <v>8.416783095802412e-05</v>
       </c>
       <c r="O30" t="n">
-        <v>0.003274872036266791</v>
+        <v>9.983770403743381e-05</v>
       </c>
       <c r="P30" t="n">
-        <v>0.003767252942236205</v>
+        <v>0.0001177651907423844</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.004268960456163219</v>
+        <v>0.0001378475985844266</v>
       </c>
       <c r="R30" t="n">
-        <v>0.004774963578196031</v>
+        <v>0.000159987291923164</v>
       </c>
       <c r="S30" t="n">
-        <v>0.005281572169687525</v>
+        <v>0.000184091398616713</v>
       </c>
       <c r="T30" t="n">
-        <v>0.0057860718725297</v>
+        <v>0.0002100715365943626</v>
       </c>
       <c r="U30" t="n">
-        <v>0.006286467050774892</v>
+        <v>0.0002378435587943859</v>
       </c>
       <c r="V30" t="n">
-        <v>0.006781296896984843</v>
+        <v>0.0002673273150476659</v>
       </c>
       <c r="W30" t="n">
-        <v>0.007269502024570764</v>
+        <v>0.000298446429611951</v>
       </c>
       <c r="X30" t="n">
-        <v>0.007750326479523362</v>
+        <v>0.0003311280931736055</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.008223244972998232</v>
+        <v>0.0003653028682349371</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.008687908314140808</v>
+        <v>0.0004009045068966862</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.009144102136023268</v>
+        <v>0.0004378697801282196</v>
       </c>
       <c r="AB30" t="n">
-        <v>0.009591715437046627</v>
+        <v>0.0004761383176932017</v>
       </c>
       <c r="AC30" t="n">
-        <v>0.01003071644196969</v>
+        <v>0.0005156524579665525</v>
       </c>
       <c r="AD30" t="n">
-        <v>0.01046113397060105</v>
+        <v>0.0005563571069406424</v>
       </c>
       <c r="AE30" t="n">
-        <v>0.01088304298471667</v>
+        <v>0.0005981996057750502</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>259</v>
+        <v>150</v>
       </c>
       <c r="B31" t="n">
-        <v>0.02429995073159442</v>
+        <v>0.0001083234633310432</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01213642713730154</v>
+        <v>8.961078278904814e-05</v>
       </c>
       <c r="D31" t="n">
-        <v>0.006563407218937635</v>
+        <v>7.485179470990333e-05</v>
       </c>
       <c r="E31" t="n">
-        <v>0.003757400153237373</v>
+        <v>6.385256582333809e-05</v>
       </c>
       <c r="F31" t="n">
-        <v>0.002302721712463175</v>
+        <v>5.643001699748374e-05</v>
       </c>
       <c r="G31" t="n">
-        <v>0.001592268319684974</v>
+        <v>5.241119785848411e-05</v>
       </c>
       <c r="H31" t="n">
-        <v>0.001324618124644319</v>
+        <v>5.163261843728564e-05</v>
       </c>
       <c r="I31" t="n">
-        <v>0.00133425841078325</v>
+        <v>5.39396326758079e-05</v>
       </c>
       <c r="J31" t="n">
-        <v>0.001523533339350018</v>
+        <v>5.918586915476817e-05</v>
       </c>
       <c r="K31" t="n">
-        <v>0.001831668757956038</v>
+        <v>6.723270487485936e-05</v>
       </c>
       <c r="L31" t="n">
-        <v>0.00221927177945759</v>
+        <v>7.794877833948566e-05</v>
       </c>
       <c r="M31" t="n">
-        <v>0.002659986723101992</v>
+        <v>9.120953855739935e-05</v>
       </c>
       <c r="N31" t="n">
-        <v>0.003135735782001965</v>
+        <v>0.0001068968269128528</v>
       </c>
       <c r="O31" t="n">
-        <v>0.00363387383237574</v>
+        <v>0.0001248984891445034</v>
       </c>
       <c r="P31" t="n">
-        <v>0.004145420188937293</v>
+        <v>0.0001451080149364793</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.004663923245044661</v>
+        <v>0.0001674242028591997</v>
       </c>
       <c r="R31" t="n">
-        <v>0.00518471098791265</v>
+        <v>0.000191750848607552</v>
       </c>
       <c r="S31" t="n">
-        <v>0.005704384321270802</v>
+        <v>0.000217996454671781</v>
       </c>
       <c r="T31" t="n">
-        <v>0.006220467397826561</v>
+        <v>0.0002460739597457384</v>
       </c>
       <c r="U31" t="n">
-        <v>0.006731161928809667</v>
+        <v>0.0002759004863285975</v>
       </c>
       <c r="V31" t="n">
-        <v>0.007235171808999553</v>
+        <v>0.0003073971051128831</v>
       </c>
       <c r="W31" t="n">
-        <v>0.007731576184083408</v>
+        <v>0.0003404886148749725</v>
       </c>
       <c r="X31" t="n">
-        <v>0.00821973644748299</v>
+        <v>0.0003751033366950724</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.008699227355732964</v>
+        <v>0.0004111729214343398</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.009169785517628211</v>
+        <v>0.0004486321694873415</v>
       </c>
       <c r="AA31" t="n">
-        <v>0.009631270549252918</v>
+        <v>0.0004874188619107361</v>
       </c>
       <c r="AB31" t="n">
-        <v>0.01008363556313318</v>
+        <v>0.0005274736021028685</v>
       </c>
       <c r="AC31" t="n">
-        <v>0.01052690460384311</v>
+        <v>0.0005687396672775767</v>
       </c>
       <c r="AD31" t="n">
-        <v>0.01096115529922496</v>
+        <v>0.0006111628690359826</v>
       </c>
       <c r="AE31" t="n">
-        <v>0.01138650545927603</v>
+        <v>0.0006546914223967282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>